<commit_message>
lista de verificacion v1.2
</commit_message>
<xml_diff>
--- a/DOCUMENTATION/G3_Lista De VerificacionISOIEC29119 2007.xlsx
+++ b/DOCUMENTATION/G3_Lista De VerificacionISOIEC29119 2007.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\UNIVERSIDAD\Aseguramiento de la Calidad del Software\Segundo Parcial\15390_G3_ACSW\DOCUMENTATION\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984E227A-78B5-4CB2-9BDC-629D06AE759C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAEBBE6-859F-411E-A3B3-15677C15A926}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="2" xr2:uid="{AA0757F3-7C9A-43E8-AE92-280E31840668}"/>
   </bookViews>
@@ -379,28 +379,6 @@
     <t>Grupo 3</t>
   </si>
   <si>
-    <t>The tester will determine expected results and implement checks or feedback on results using keywords.
-Keywords can be used to check the results the test item returns and log them accordingly</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The result is then checked by one or more other actions i.e. the verification steps. </t>
-  </si>
-  <si>
-    <t>interface to the test item used to stimulate the test item, to get responses (e.g. actual results), or both</t>
-  </si>
-  <si>
-    <t>The tester selects input values based on test design considerations and then implements these in keywords. In situations where test cases are supposed to be executed according to the same actions, but with different sets of data to provide different test outcomes, the keywords will normally be developed to support data-driven
-testing</t>
-  </si>
-  <si>
-    <t>The tester determines and establishes the needed test pre-conditions and identifies which can be achieved
-using keywords or other actions. Composite high-level keywords (see 5.3.2) can be appropriate in a situation
-where multiple actions are required</t>
-  </si>
-  <si>
-    <t>Within the test case specification (see ISO/IEC/IEEE 29119-3), test cases can be documented using appropriate notation, including the use of tables or databases. The format depends on the available infrastructure</t>
-  </si>
-  <si>
     <t xml:space="preserve">4.13 test interface 
 6.6.5.3 Select input values
  </t>
@@ -426,6 +404,24 @@
   </si>
   <si>
     <t xml:space="preserve">4.13 test interface </t>
+  </si>
+  <si>
+    <t>Utiliza palabras clave para comprobar los resultados que devuelve el elemento de prueba y registrarlos en consecuencia?</t>
+  </si>
+  <si>
+    <t>Cuenta con los anexos correspondientes dentro de las pruebas de caja negra?</t>
+  </si>
+  <si>
+    <t>La funcionalidad y la integridad de la interfaz es amigable durante el desarrollo de las pruebas ?</t>
+  </si>
+  <si>
+    <t>Dentro de las pruebas de caja Blanca y caja negra los valores seleccionados para las mismas son claros, correctos y probables?</t>
+  </si>
+  <si>
+    <t>Dentro de la documentacion se puede evidenciar las precondiciones de cada requisito que se desarrollo?</t>
+  </si>
+  <si>
+    <t>Se realizaron casos de pruebas a cada requisito entregado durante la revisison?</t>
   </si>
 </sst>
 </file>
@@ -1620,14 +1616,44 @@
     <xf numFmtId="0" fontId="23" fillId="8" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1641,8 +1667,32 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="2" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="3" xfId="11" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="0" borderId="5" xfId="11" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1650,173 +1700,119 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="31" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="11" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="5" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="31" xfId="11" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="32" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="32" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="22" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="31" xfId="11" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="32" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="31" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="11" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="32" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="2" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="3" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="5" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="2" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="2" xfId="11" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="3" xfId="11" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="5" xfId="11" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="11" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="12" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2148,8 +2144,8 @@
   </sheetPr>
   <dimension ref="B1:J10"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2178,7 +2174,7 @@
     </row>
     <row r="2" spans="2:10" ht="24" customHeight="1">
       <c r="B2" s="81" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C2" s="81"/>
       <c r="D2" s="81"/>
@@ -2236,7 +2232,7 @@
       </c>
       <c r="F5" s="89"/>
       <c r="G5" s="90" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="H5" s="91"/>
       <c r="I5" s="92"/>
@@ -2377,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC422AF-D626-4C6F-A609-BD2ACA92CE0C}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="E16" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" topLeftCell="B13" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -2614,7 +2610,7 @@
         <v>33</v>
       </c>
       <c r="H16" s="59" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I16" s="55"/>
     </row>
@@ -2693,7 +2689,7 @@
         <v>33</v>
       </c>
       <c r="H19" s="62" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="I19" s="56"/>
     </row>
@@ -2762,7 +2758,7 @@
         <v>33</v>
       </c>
       <c r="H22" s="60" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="I22" s="56"/>
     </row>
@@ -2814,7 +2810,7 @@
         <v>33</v>
       </c>
       <c r="H24" s="59" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="I24" s="57"/>
     </row>
@@ -2866,7 +2862,7 @@
         <v>33</v>
       </c>
       <c r="H26" s="60" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="I26" s="56" t="s">
         <v>96</v>
@@ -2987,7 +2983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3958C6-2939-4E23-8274-C21200294795}">
   <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="75" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="110" zoomScaleNormal="75" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="D13" sqref="D13:K13"/>
     </sheetView>
   </sheetViews>
@@ -3006,121 +3002,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="33" customHeight="1">
-      <c r="A1" s="125"/>
-      <c r="B1" s="125"/>
-      <c r="C1" s="134" t="s">
+      <c r="A1" s="114"/>
+      <c r="B1" s="114"/>
+      <c r="C1" s="149" t="s">
         <v>68</v>
       </c>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
-      <c r="K1" s="135"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
-      <c r="N1" s="135"/>
-      <c r="O1" s="136"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="150"/>
+      <c r="K1" s="150"/>
+      <c r="L1" s="150"/>
+      <c r="M1" s="150"/>
+      <c r="N1" s="150"/>
+      <c r="O1" s="151"/>
       <c r="P1" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="127" t="s">
+      <c r="Q1" s="142" t="s">
         <v>70</v>
       </c>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="129"/>
+      <c r="R1" s="143"/>
+      <c r="S1" s="143"/>
+      <c r="T1" s="144"/>
     </row>
     <row r="2" spans="1:20" ht="30.95" customHeight="1">
-      <c r="A2" s="125"/>
-      <c r="B2" s="125"/>
-      <c r="C2" s="137" t="s">
+      <c r="A2" s="114"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="152" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="139"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
+      <c r="J2" s="153"/>
+      <c r="K2" s="153"/>
+      <c r="L2" s="153"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="153"/>
+      <c r="O2" s="154"/>
       <c r="P2" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" s="127" t="s">
+      <c r="Q2" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="R2" s="128"/>
-      <c r="S2" s="128"/>
-      <c r="T2" s="129"/>
+      <c r="R2" s="143"/>
+      <c r="S2" s="143"/>
+      <c r="T2" s="144"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1">
-      <c r="A3" s="133" t="s">
+      <c r="A3" s="148" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="133"/>
-      <c r="C3" s="140" t="s">
+      <c r="B3" s="148"/>
+      <c r="C3" s="155" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="141"/>
-      <c r="E3" s="141"/>
-      <c r="F3" s="141"/>
-      <c r="G3" s="141"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="141"/>
-      <c r="J3" s="141"/>
-      <c r="K3" s="141"/>
-      <c r="L3" s="141"/>
-      <c r="M3" s="141"/>
-      <c r="N3" s="141"/>
-      <c r="O3" s="142"/>
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="I3" s="156"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="156"/>
+      <c r="L3" s="156"/>
+      <c r="M3" s="156"/>
+      <c r="N3" s="156"/>
+      <c r="O3" s="157"/>
       <c r="P3" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="Q3" s="130" t="s">
+      <c r="Q3" s="145" t="s">
         <v>77</v>
       </c>
-      <c r="R3" s="131"/>
-      <c r="S3" s="131"/>
-      <c r="T3" s="132"/>
+      <c r="R3" s="146"/>
+      <c r="S3" s="146"/>
+      <c r="T3" s="147"/>
     </row>
     <row r="4" spans="1:20" ht="12" customHeight="1">
       <c r="A4" s="37"/>
     </row>
     <row r="5" spans="1:20" ht="49.5" customHeight="1">
-      <c r="A5" s="110" t="s">
+      <c r="A5" s="128" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="161">
+      <c r="B5" s="128"/>
+      <c r="C5" s="135">
         <v>2024</v>
       </c>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="H5" s="145" t="s">
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="H5" s="158" t="s">
         <v>79</v>
       </c>
-      <c r="I5" s="146"/>
-      <c r="J5" s="159">
+      <c r="I5" s="159"/>
+      <c r="J5" s="133">
         <v>1</v>
       </c>
-      <c r="K5" s="160"/>
+      <c r="K5" s="134"/>
       <c r="P5" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="R5" s="153">
+      <c r="R5" s="125">
         <v>45336</v>
       </c>
-      <c r="S5" s="154"/>
-      <c r="T5" s="155"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="127"/>
     </row>
     <row r="6" spans="1:20" ht="18.75" customHeight="1">
       <c r="A6" s="46"/>
@@ -3128,22 +3124,22 @@
       <c r="P6" s="46"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="128" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="143" t="s">
+      <c r="B7" s="129"/>
+      <c r="C7" s="123" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="144"/>
+      <c r="D7" s="124"/>
+      <c r="E7" s="124"/>
+      <c r="F7" s="124"/>
+      <c r="G7" s="124"/>
+      <c r="H7" s="124"/>
+      <c r="I7" s="124"/>
+      <c r="J7" s="124"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="124"/>
       <c r="P7" s="46" t="s">
         <v>83</v>
       </c>
@@ -3162,22 +3158,22 @@
       <c r="A8" s="46"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="110" t="s">
+      <c r="A9" s="128" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="111"/>
-      <c r="C9" s="143" t="s">
+      <c r="B9" s="129"/>
+      <c r="C9" s="123" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="144"/>
-      <c r="E9" s="144"/>
-      <c r="F9" s="144"/>
-      <c r="G9" s="144"/>
-      <c r="H9" s="144"/>
-      <c r="I9" s="144"/>
-      <c r="J9" s="144"/>
-      <c r="K9" s="144"/>
-      <c r="L9" s="144"/>
+      <c r="D9" s="124"/>
+      <c r="E9" s="124"/>
+      <c r="F9" s="124"/>
+      <c r="G9" s="124"/>
+      <c r="H9" s="124"/>
+      <c r="I9" s="124"/>
+      <c r="J9" s="124"/>
+      <c r="K9" s="124"/>
+      <c r="L9" s="124"/>
       <c r="P9" s="45"/>
       <c r="Q9" s="39"/>
       <c r="R9" s="39"/>
@@ -3195,1138 +3191,1269 @@
       <c r="A11" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="119" t="s">
+      <c r="C11" s="161"/>
+      <c r="D11" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="E11" s="120"/>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="120"/>
-      <c r="J11" s="120"/>
-      <c r="K11" s="121"/>
-      <c r="L11" s="119" t="s">
+      <c r="E11" s="137"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="137"/>
+      <c r="I11" s="137"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="162"/>
+      <c r="L11" s="136" t="s">
         <v>89</v>
       </c>
-      <c r="M11" s="120"/>
-      <c r="N11" s="120"/>
-      <c r="O11" s="120"/>
-      <c r="P11" s="120"/>
-      <c r="Q11" s="120"/>
-      <c r="R11" s="120"/>
-      <c r="S11" s="120"/>
-      <c r="T11" s="162"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="137"/>
+      <c r="O11" s="137"/>
+      <c r="P11" s="137"/>
+      <c r="Q11" s="137"/>
+      <c r="R11" s="137"/>
+      <c r="S11" s="137"/>
+      <c r="T11" s="138"/>
     </row>
     <row r="12" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A12" s="41">
         <v>1</v>
       </c>
-      <c r="B12" s="147" t="s">
+      <c r="B12" s="121" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="148"/>
-      <c r="D12" s="156" t="s">
-        <v>102</v>
-      </c>
-      <c r="E12" s="157"/>
-      <c r="F12" s="157"/>
-      <c r="G12" s="157"/>
-      <c r="H12" s="157"/>
-      <c r="I12" s="157"/>
-      <c r="J12" s="157"/>
-      <c r="K12" s="158"/>
-      <c r="L12" s="147"/>
-      <c r="M12" s="148"/>
-      <c r="N12" s="148"/>
-      <c r="O12" s="148"/>
-      <c r="P12" s="148"/>
-      <c r="Q12" s="148"/>
-      <c r="R12" s="148"/>
-      <c r="S12" s="148"/>
-      <c r="T12" s="149"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="130" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="131"/>
+      <c r="F12" s="131"/>
+      <c r="G12" s="131"/>
+      <c r="H12" s="131"/>
+      <c r="I12" s="131"/>
+      <c r="J12" s="131"/>
+      <c r="K12" s="132"/>
+      <c r="L12" s="121"/>
+      <c r="M12" s="104"/>
+      <c r="N12" s="104"/>
+      <c r="O12" s="104"/>
+      <c r="P12" s="104"/>
+      <c r="Q12" s="104"/>
+      <c r="R12" s="104"/>
+      <c r="S12" s="104"/>
+      <c r="T12" s="122"/>
     </row>
     <row r="13" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A13" s="40">
         <v>2</v>
       </c>
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="113" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="114"/>
+      <c r="D13" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="C13" s="125"/>
-      <c r="D13" s="115" t="s">
-        <v>103</v>
-      </c>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
-      <c r="L13" s="115"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="116"/>
-      <c r="O13" s="116"/>
-      <c r="P13" s="116"/>
-      <c r="Q13" s="116"/>
-      <c r="R13" s="116"/>
-      <c r="S13" s="116"/>
-      <c r="T13" s="150"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="106"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="106"/>
+      <c r="N13" s="106"/>
+      <c r="O13" s="106"/>
+      <c r="P13" s="106"/>
+      <c r="Q13" s="106"/>
+      <c r="R13" s="106"/>
+      <c r="S13" s="106"/>
+      <c r="T13" s="107"/>
     </row>
     <row r="14" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A14" s="41">
         <v>3</v>
       </c>
-      <c r="B14" s="148" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="148"/>
-      <c r="D14" s="163" t="s">
-        <v>104</v>
-      </c>
-      <c r="E14" s="164"/>
-      <c r="F14" s="164"/>
-      <c r="G14" s="164"/>
-      <c r="H14" s="164"/>
-      <c r="I14" s="164"/>
-      <c r="J14" s="164"/>
-      <c r="K14" s="165"/>
-      <c r="L14" s="115"/>
-      <c r="M14" s="116"/>
-      <c r="N14" s="116"/>
-      <c r="O14" s="116"/>
-      <c r="P14" s="116"/>
-      <c r="Q14" s="116"/>
-      <c r="R14" s="116"/>
-      <c r="S14" s="116"/>
-      <c r="T14" s="150"/>
+      <c r="B14" s="104" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="104"/>
+      <c r="D14" s="139" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="140"/>
+      <c r="F14" s="140"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="140"/>
+      <c r="J14" s="140"/>
+      <c r="K14" s="141"/>
+      <c r="L14" s="105"/>
+      <c r="M14" s="106"/>
+      <c r="N14" s="106"/>
+      <c r="O14" s="106"/>
+      <c r="P14" s="106"/>
+      <c r="Q14" s="106"/>
+      <c r="R14" s="106"/>
+      <c r="S14" s="106"/>
+      <c r="T14" s="107"/>
     </row>
     <row r="15" spans="1:20" s="42" customFormat="1" ht="96.95" customHeight="1" thickBot="1">
       <c r="A15" s="40">
         <v>4</v>
       </c>
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="106" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="116"/>
-      <c r="D15" s="115" t="s">
-        <v>105</v>
-      </c>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
-      <c r="G15" s="116"/>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="116"/>
-      <c r="L15" s="126"/>
-      <c r="M15" s="151"/>
-      <c r="N15" s="151"/>
-      <c r="O15" s="151"/>
-      <c r="P15" s="151"/>
-      <c r="Q15" s="151"/>
-      <c r="R15" s="151"/>
-      <c r="S15" s="151"/>
-      <c r="T15" s="152"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="106"/>
+      <c r="F15" s="106"/>
+      <c r="G15" s="106"/>
+      <c r="H15" s="106"/>
+      <c r="I15" s="106"/>
+      <c r="J15" s="106"/>
+      <c r="K15" s="106"/>
+      <c r="L15" s="108"/>
+      <c r="M15" s="110"/>
+      <c r="N15" s="110"/>
+      <c r="O15" s="110"/>
+      <c r="P15" s="110"/>
+      <c r="Q15" s="110"/>
+      <c r="R15" s="110"/>
+      <c r="S15" s="110"/>
+      <c r="T15" s="111"/>
     </row>
     <row r="16" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A16" s="40">
         <v>5</v>
       </c>
-      <c r="B16" s="148" t="s">
+      <c r="B16" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="122"/>
-      <c r="D16" s="116" t="s">
-        <v>106</v>
-      </c>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="116"/>
-      <c r="L16" s="116"/>
-      <c r="M16" s="116"/>
-      <c r="N16" s="116"/>
-      <c r="O16" s="116"/>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="116"/>
-      <c r="S16" s="116"/>
-      <c r="T16" s="150"/>
+      <c r="C16" s="119"/>
+      <c r="D16" s="106" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="106"/>
+      <c r="F16" s="106"/>
+      <c r="G16" s="106"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="106"/>
+      <c r="M16" s="106"/>
+      <c r="N16" s="106"/>
+      <c r="O16" s="106"/>
+      <c r="P16" s="106"/>
+      <c r="Q16" s="106"/>
+      <c r="R16" s="106"/>
+      <c r="S16" s="106"/>
+      <c r="T16" s="107"/>
     </row>
     <row r="17" spans="1:20" s="42" customFormat="1" ht="78.75" customHeight="1">
       <c r="A17" s="41">
         <v>6</v>
       </c>
-      <c r="B17" s="116" t="s">
-        <v>114</v>
-      </c>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="116"/>
-      <c r="L17" s="116"/>
-      <c r="M17" s="116"/>
-      <c r="N17" s="116"/>
-      <c r="O17" s="116"/>
-      <c r="P17" s="116"/>
-      <c r="Q17" s="116"/>
-      <c r="R17" s="116"/>
-      <c r="S17" s="116"/>
-      <c r="T17" s="150"/>
+      <c r="B17" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="106"/>
+      <c r="F17" s="106"/>
+      <c r="G17" s="106"/>
+      <c r="H17" s="106"/>
+      <c r="I17" s="106"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="106"/>
+      <c r="M17" s="106"/>
+      <c r="N17" s="106"/>
+      <c r="O17" s="106"/>
+      <c r="P17" s="106"/>
+      <c r="Q17" s="106"/>
+      <c r="R17" s="106"/>
+      <c r="S17" s="106"/>
+      <c r="T17" s="107"/>
     </row>
     <row r="18" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A18" s="40">
         <v>7</v>
       </c>
-      <c r="B18" s="166"/>
-      <c r="C18" s="166"/>
-      <c r="D18" s="126"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="123"/>
-      <c r="K18" s="123"/>
-      <c r="L18" s="151"/>
-      <c r="M18" s="151"/>
-      <c r="N18" s="151"/>
-      <c r="O18" s="151"/>
-      <c r="P18" s="151"/>
-      <c r="Q18" s="151"/>
-      <c r="R18" s="151"/>
-      <c r="S18" s="151"/>
-      <c r="T18" s="152"/>
+      <c r="B18" s="120"/>
+      <c r="C18" s="120"/>
+      <c r="D18" s="108"/>
+      <c r="E18" s="109"/>
+      <c r="F18" s="109"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="109"/>
+      <c r="K18" s="109"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="110"/>
+      <c r="N18" s="110"/>
+      <c r="O18" s="110"/>
+      <c r="P18" s="110"/>
+      <c r="Q18" s="110"/>
+      <c r="R18" s="110"/>
+      <c r="S18" s="110"/>
+      <c r="T18" s="111"/>
     </row>
     <row r="19" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A19" s="41">
         <v>8</v>
       </c>
-      <c r="B19" s="124"/>
-      <c r="C19" s="125"/>
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="123"/>
-      <c r="J19" s="123"/>
-      <c r="K19" s="123"/>
-      <c r="L19" s="151"/>
-      <c r="M19" s="151"/>
-      <c r="N19" s="151"/>
-      <c r="O19" s="151"/>
-      <c r="P19" s="151"/>
-      <c r="Q19" s="151"/>
-      <c r="R19" s="151"/>
-      <c r="S19" s="151"/>
-      <c r="T19" s="152"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="114"/>
+      <c r="D19" s="109"/>
+      <c r="E19" s="109"/>
+      <c r="F19" s="109"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="109"/>
+      <c r="K19" s="109"/>
+      <c r="L19" s="110"/>
+      <c r="M19" s="110"/>
+      <c r="N19" s="110"/>
+      <c r="O19" s="110"/>
+      <c r="P19" s="110"/>
+      <c r="Q19" s="110"/>
+      <c r="R19" s="110"/>
+      <c r="S19" s="110"/>
+      <c r="T19" s="111"/>
     </row>
     <row r="20" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A20" s="40">
         <v>9</v>
       </c>
-      <c r="B20" s="124"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
-      <c r="F20" s="123"/>
-      <c r="G20" s="123"/>
-      <c r="H20" s="123"/>
-      <c r="I20" s="123"/>
-      <c r="J20" s="123"/>
-      <c r="K20" s="123"/>
-      <c r="L20" s="151"/>
-      <c r="M20" s="151"/>
-      <c r="N20" s="151"/>
-      <c r="O20" s="151"/>
-      <c r="P20" s="151"/>
-      <c r="Q20" s="151"/>
-      <c r="R20" s="151"/>
-      <c r="S20" s="151"/>
-      <c r="T20" s="152"/>
+      <c r="B20" s="113"/>
+      <c r="C20" s="114"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="109"/>
+      <c r="G20" s="109"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="110"/>
+      <c r="M20" s="110"/>
+      <c r="N20" s="110"/>
+      <c r="O20" s="110"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="110"/>
+      <c r="S20" s="110"/>
+      <c r="T20" s="111"/>
     </row>
     <row r="21" spans="1:20" s="42" customFormat="1" ht="87" customHeight="1" thickBot="1">
       <c r="A21" s="40">
         <v>10</v>
       </c>
-      <c r="B21" s="124"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="126"/>
-      <c r="E21" s="123"/>
-      <c r="F21" s="123"/>
-      <c r="G21" s="123"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="123"/>
-      <c r="J21" s="123"/>
-      <c r="K21" s="123"/>
-      <c r="L21" s="151"/>
-      <c r="M21" s="151"/>
-      <c r="N21" s="151"/>
-      <c r="O21" s="151"/>
-      <c r="P21" s="151"/>
-      <c r="Q21" s="151"/>
-      <c r="R21" s="151"/>
-      <c r="S21" s="151"/>
-      <c r="T21" s="152"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="110"/>
+      <c r="N21" s="110"/>
+      <c r="O21" s="110"/>
+      <c r="P21" s="110"/>
+      <c r="Q21" s="110"/>
+      <c r="R21" s="110"/>
+      <c r="S21" s="110"/>
+      <c r="T21" s="111"/>
     </row>
     <row r="22" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A22" s="41">
         <v>11</v>
       </c>
-      <c r="B22" s="124"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="126"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="123"/>
-      <c r="I22" s="123"/>
-      <c r="J22" s="123"/>
-      <c r="K22" s="123"/>
-      <c r="L22" s="167"/>
-      <c r="M22" s="151"/>
-      <c r="N22" s="151"/>
-      <c r="O22" s="151"/>
-      <c r="P22" s="151"/>
-      <c r="Q22" s="151"/>
-      <c r="R22" s="151"/>
-      <c r="S22" s="151"/>
-      <c r="T22" s="152"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="114"/>
+      <c r="D22" s="108"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="109"/>
+      <c r="G22" s="109"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="112"/>
+      <c r="M22" s="110"/>
+      <c r="N22" s="110"/>
+      <c r="O22" s="110"/>
+      <c r="P22" s="110"/>
+      <c r="Q22" s="110"/>
+      <c r="R22" s="110"/>
+      <c r="S22" s="110"/>
+      <c r="T22" s="111"/>
     </row>
     <row r="23" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A23" s="40">
         <v>12</v>
       </c>
-      <c r="B23" s="124"/>
-      <c r="C23" s="125"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="123"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="123"/>
-      <c r="K23" s="123"/>
-      <c r="L23" s="151"/>
-      <c r="M23" s="151"/>
-      <c r="N23" s="151"/>
-      <c r="O23" s="151"/>
-      <c r="P23" s="151"/>
-      <c r="Q23" s="151"/>
-      <c r="R23" s="151"/>
-      <c r="S23" s="151"/>
-      <c r="T23" s="152"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="114"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="110"/>
+      <c r="M23" s="110"/>
+      <c r="N23" s="110"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="110"/>
+      <c r="Q23" s="110"/>
+      <c r="R23" s="110"/>
+      <c r="S23" s="110"/>
+      <c r="T23" s="111"/>
     </row>
     <row r="24" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A24" s="41">
         <v>13</v>
       </c>
-      <c r="B24" s="124"/>
-      <c r="C24" s="125"/>
-      <c r="D24" s="126"/>
-      <c r="E24" s="123"/>
-      <c r="F24" s="123"/>
-      <c r="G24" s="123"/>
-      <c r="H24" s="123"/>
-      <c r="I24" s="123"/>
-      <c r="J24" s="123"/>
-      <c r="K24" s="123"/>
-      <c r="L24" s="151"/>
-      <c r="M24" s="151"/>
-      <c r="N24" s="151"/>
-      <c r="O24" s="151"/>
-      <c r="P24" s="151"/>
-      <c r="Q24" s="151"/>
-      <c r="R24" s="151"/>
-      <c r="S24" s="151"/>
-      <c r="T24" s="152"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="108"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="109"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="109"/>
+      <c r="K24" s="109"/>
+      <c r="L24" s="110"/>
+      <c r="M24" s="110"/>
+      <c r="N24" s="110"/>
+      <c r="O24" s="110"/>
+      <c r="P24" s="110"/>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="110"/>
+      <c r="S24" s="110"/>
+      <c r="T24" s="111"/>
     </row>
     <row r="25" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A25" s="40">
         <v>14</v>
       </c>
-      <c r="B25" s="124"/>
-      <c r="C25" s="125"/>
-      <c r="D25" s="126"/>
-      <c r="E25" s="123"/>
-      <c r="F25" s="123"/>
-      <c r="G25" s="123"/>
-      <c r="H25" s="123"/>
-      <c r="I25" s="123"/>
-      <c r="J25" s="123"/>
-      <c r="K25" s="123"/>
-      <c r="L25" s="151"/>
-      <c r="M25" s="151"/>
-      <c r="N25" s="151"/>
-      <c r="O25" s="151"/>
-      <c r="P25" s="151"/>
-      <c r="Q25" s="151"/>
-      <c r="R25" s="151"/>
-      <c r="S25" s="151"/>
-      <c r="T25" s="152"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="114"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
+      <c r="J25" s="109"/>
+      <c r="K25" s="109"/>
+      <c r="L25" s="110"/>
+      <c r="M25" s="110"/>
+      <c r="N25" s="110"/>
+      <c r="O25" s="110"/>
+      <c r="P25" s="110"/>
+      <c r="Q25" s="110"/>
+      <c r="R25" s="110"/>
+      <c r="S25" s="110"/>
+      <c r="T25" s="111"/>
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A26" s="40">
         <v>15</v>
       </c>
-      <c r="B26" s="124"/>
-      <c r="C26" s="125"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="123"/>
-      <c r="G26" s="123"/>
-      <c r="H26" s="123"/>
-      <c r="I26" s="123"/>
-      <c r="J26" s="123"/>
-      <c r="K26" s="123"/>
-      <c r="L26" s="151"/>
-      <c r="M26" s="151"/>
-      <c r="N26" s="151"/>
-      <c r="O26" s="151"/>
-      <c r="P26" s="151"/>
-      <c r="Q26" s="151"/>
-      <c r="R26" s="151"/>
-      <c r="S26" s="151"/>
-      <c r="T26" s="152"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="114"/>
+      <c r="D26" s="109"/>
+      <c r="E26" s="109"/>
+      <c r="F26" s="109"/>
+      <c r="G26" s="109"/>
+      <c r="H26" s="109"/>
+      <c r="I26" s="109"/>
+      <c r="J26" s="109"/>
+      <c r="K26" s="109"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="110"/>
+      <c r="N26" s="110"/>
+      <c r="O26" s="110"/>
+      <c r="P26" s="110"/>
+      <c r="Q26" s="110"/>
+      <c r="R26" s="110"/>
+      <c r="S26" s="110"/>
+      <c r="T26" s="111"/>
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A27" s="41">
         <v>16</v>
       </c>
-      <c r="B27" s="124"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="126"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="123"/>
-      <c r="I27" s="123"/>
-      <c r="J27" s="123"/>
-      <c r="K27" s="123"/>
-      <c r="L27" s="151"/>
-      <c r="M27" s="151"/>
-      <c r="N27" s="151"/>
-      <c r="O27" s="151"/>
-      <c r="P27" s="151"/>
-      <c r="Q27" s="151"/>
-      <c r="R27" s="151"/>
-      <c r="S27" s="151"/>
-      <c r="T27" s="152"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="114"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="110"/>
+      <c r="M27" s="110"/>
+      <c r="N27" s="110"/>
+      <c r="O27" s="110"/>
+      <c r="P27" s="110"/>
+      <c r="Q27" s="110"/>
+      <c r="R27" s="110"/>
+      <c r="S27" s="110"/>
+      <c r="T27" s="111"/>
     </row>
     <row r="28" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A28" s="40">
         <v>17</v>
       </c>
-      <c r="B28" s="124"/>
-      <c r="C28" s="125"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="123"/>
-      <c r="G28" s="123"/>
-      <c r="H28" s="123"/>
-      <c r="I28" s="123"/>
-      <c r="J28" s="123"/>
-      <c r="K28" s="123"/>
-      <c r="L28" s="151"/>
-      <c r="M28" s="151"/>
-      <c r="N28" s="151"/>
-      <c r="O28" s="151"/>
-      <c r="P28" s="151"/>
-      <c r="Q28" s="151"/>
-      <c r="R28" s="151"/>
-      <c r="S28" s="151"/>
-      <c r="T28" s="152"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="108"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="109"/>
+      <c r="H28" s="109"/>
+      <c r="I28" s="109"/>
+      <c r="J28" s="109"/>
+      <c r="K28" s="109"/>
+      <c r="L28" s="110"/>
+      <c r="M28" s="110"/>
+      <c r="N28" s="110"/>
+      <c r="O28" s="110"/>
+      <c r="P28" s="110"/>
+      <c r="Q28" s="110"/>
+      <c r="R28" s="110"/>
+      <c r="S28" s="110"/>
+      <c r="T28" s="111"/>
     </row>
     <row r="29" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A29" s="41">
         <v>18</v>
       </c>
-      <c r="B29" s="124"/>
-      <c r="C29" s="125"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="123"/>
-      <c r="F29" s="123"/>
-      <c r="G29" s="123"/>
-      <c r="H29" s="123"/>
-      <c r="I29" s="123"/>
-      <c r="J29" s="123"/>
-      <c r="K29" s="123"/>
-      <c r="L29" s="151"/>
-      <c r="M29" s="151"/>
-      <c r="N29" s="151"/>
-      <c r="O29" s="151"/>
-      <c r="P29" s="151"/>
-      <c r="Q29" s="151"/>
-      <c r="R29" s="151"/>
-      <c r="S29" s="151"/>
-      <c r="T29" s="152"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="114"/>
+      <c r="D29" s="108"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="109"/>
+      <c r="H29" s="109"/>
+      <c r="I29" s="109"/>
+      <c r="J29" s="109"/>
+      <c r="K29" s="109"/>
+      <c r="L29" s="110"/>
+      <c r="M29" s="110"/>
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="110"/>
+      <c r="R29" s="110"/>
+      <c r="S29" s="110"/>
+      <c r="T29" s="111"/>
     </row>
     <row r="30" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A30" s="40">
         <v>19</v>
       </c>
-      <c r="B30" s="124"/>
-      <c r="C30" s="125"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="123"/>
-      <c r="I30" s="123"/>
-      <c r="J30" s="123"/>
-      <c r="K30" s="123"/>
-      <c r="L30" s="151"/>
-      <c r="M30" s="151"/>
-      <c r="N30" s="151"/>
-      <c r="O30" s="151"/>
-      <c r="P30" s="151"/>
-      <c r="Q30" s="151"/>
-      <c r="R30" s="151"/>
-      <c r="S30" s="151"/>
-      <c r="T30" s="152"/>
+      <c r="B30" s="113"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="109"/>
+      <c r="H30" s="109"/>
+      <c r="I30" s="109"/>
+      <c r="J30" s="109"/>
+      <c r="K30" s="109"/>
+      <c r="L30" s="110"/>
+      <c r="M30" s="110"/>
+      <c r="N30" s="110"/>
+      <c r="O30" s="110"/>
+      <c r="P30" s="110"/>
+      <c r="Q30" s="110"/>
+      <c r="R30" s="110"/>
+      <c r="S30" s="110"/>
+      <c r="T30" s="111"/>
     </row>
     <row r="31" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A31" s="40">
         <v>20</v>
       </c>
-      <c r="B31" s="124"/>
-      <c r="C31" s="125"/>
-      <c r="D31" s="126"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="123"/>
-      <c r="H31" s="123"/>
-      <c r="I31" s="123"/>
-      <c r="J31" s="123"/>
-      <c r="K31" s="123"/>
-      <c r="L31" s="151"/>
-      <c r="M31" s="151"/>
-      <c r="N31" s="151"/>
-      <c r="O31" s="151"/>
-      <c r="P31" s="151"/>
-      <c r="Q31" s="151"/>
-      <c r="R31" s="151"/>
-      <c r="S31" s="151"/>
-      <c r="T31" s="152"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="114"/>
+      <c r="D31" s="108"/>
+      <c r="E31" s="109"/>
+      <c r="F31" s="109"/>
+      <c r="G31" s="109"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="109"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="110"/>
+      <c r="M31" s="110"/>
+      <c r="N31" s="110"/>
+      <c r="O31" s="110"/>
+      <c r="P31" s="110"/>
+      <c r="Q31" s="110"/>
+      <c r="R31" s="110"/>
+      <c r="S31" s="110"/>
+      <c r="T31" s="111"/>
     </row>
     <row r="32" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A32" s="41">
         <v>21</v>
       </c>
-      <c r="B32" s="124"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="126"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="123"/>
-      <c r="H32" s="123"/>
-      <c r="I32" s="123"/>
-      <c r="J32" s="123"/>
-      <c r="K32" s="123"/>
-      <c r="L32" s="151"/>
-      <c r="M32" s="151"/>
-      <c r="N32" s="151"/>
-      <c r="O32" s="151"/>
-      <c r="P32" s="151"/>
-      <c r="Q32" s="151"/>
-      <c r="R32" s="151"/>
-      <c r="S32" s="151"/>
-      <c r="T32" s="152"/>
+      <c r="B32" s="113"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="108"/>
+      <c r="E32" s="109"/>
+      <c r="F32" s="109"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="109"/>
+      <c r="I32" s="109"/>
+      <c r="J32" s="109"/>
+      <c r="K32" s="109"/>
+      <c r="L32" s="110"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
+      <c r="O32" s="110"/>
+      <c r="P32" s="110"/>
+      <c r="Q32" s="110"/>
+      <c r="R32" s="110"/>
+      <c r="S32" s="110"/>
+      <c r="T32" s="111"/>
     </row>
     <row r="33" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A33" s="40">
         <v>22</v>
       </c>
-      <c r="B33" s="124"/>
-      <c r="C33" s="125"/>
-      <c r="D33" s="126"/>
-      <c r="E33" s="123"/>
-      <c r="F33" s="123"/>
-      <c r="G33" s="123"/>
-      <c r="H33" s="123"/>
-      <c r="I33" s="123"/>
-      <c r="J33" s="123"/>
-      <c r="K33" s="123"/>
-      <c r="L33" s="151"/>
-      <c r="M33" s="151"/>
-      <c r="N33" s="151"/>
-      <c r="O33" s="151"/>
-      <c r="P33" s="151"/>
-      <c r="Q33" s="151"/>
-      <c r="R33" s="151"/>
-      <c r="S33" s="151"/>
-      <c r="T33" s="152"/>
+      <c r="B33" s="113"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="108"/>
+      <c r="E33" s="109"/>
+      <c r="F33" s="109"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="109"/>
+      <c r="I33" s="109"/>
+      <c r="J33" s="109"/>
+      <c r="K33" s="109"/>
+      <c r="L33" s="110"/>
+      <c r="M33" s="110"/>
+      <c r="N33" s="110"/>
+      <c r="O33" s="110"/>
+      <c r="P33" s="110"/>
+      <c r="Q33" s="110"/>
+      <c r="R33" s="110"/>
+      <c r="S33" s="110"/>
+      <c r="T33" s="111"/>
     </row>
     <row r="34" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1">
       <c r="A34" s="41">
         <v>23</v>
       </c>
-      <c r="B34" s="124"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="126"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="123"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="123"/>
-      <c r="J34" s="123"/>
-      <c r="K34" s="123"/>
-      <c r="L34" s="151"/>
-      <c r="M34" s="151"/>
-      <c r="N34" s="151"/>
-      <c r="O34" s="151"/>
-      <c r="P34" s="151"/>
-      <c r="Q34" s="151"/>
-      <c r="R34" s="151"/>
-      <c r="S34" s="151"/>
-      <c r="T34" s="152"/>
+      <c r="B34" s="113"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="108"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="110"/>
+      <c r="M34" s="110"/>
+      <c r="N34" s="110"/>
+      <c r="O34" s="110"/>
+      <c r="P34" s="110"/>
+      <c r="Q34" s="110"/>
+      <c r="R34" s="110"/>
+      <c r="S34" s="110"/>
+      <c r="T34" s="111"/>
     </row>
     <row r="35" spans="1:20" s="42" customFormat="1" ht="65.25" customHeight="1" thickBot="1">
       <c r="A35" s="40">
         <v>24</v>
       </c>
-      <c r="B35" s="105"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="107"/>
-      <c r="E35" s="108"/>
-      <c r="F35" s="108"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="108"/>
-      <c r="I35" s="108"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="112"/>
-      <c r="M35" s="112"/>
-      <c r="N35" s="112"/>
-      <c r="O35" s="112"/>
-      <c r="P35" s="112"/>
-      <c r="Q35" s="112"/>
-      <c r="R35" s="112"/>
-      <c r="S35" s="112"/>
-      <c r="T35" s="113"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="116"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="118"/>
+      <c r="F35" s="118"/>
+      <c r="G35" s="118"/>
+      <c r="H35" s="118"/>
+      <c r="I35" s="118"/>
+      <c r="J35" s="118"/>
+      <c r="K35" s="118"/>
+      <c r="L35" s="102"/>
+      <c r="M35" s="102"/>
+      <c r="N35" s="102"/>
+      <c r="O35" s="102"/>
+      <c r="P35" s="102"/>
+      <c r="Q35" s="102"/>
+      <c r="R35" s="102"/>
+      <c r="S35" s="102"/>
+      <c r="T35" s="103"/>
     </row>
     <row r="36" spans="1:20" ht="160.35" customHeight="1" thickBot="1">
       <c r="A36" s="40">
         <v>25</v>
       </c>
-      <c r="B36" s="105"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="108"/>
-      <c r="F36" s="108"/>
-      <c r="G36" s="108"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="108"/>
-      <c r="J36" s="108"/>
-      <c r="K36" s="108"/>
-      <c r="L36" s="112"/>
-      <c r="M36" s="112"/>
-      <c r="N36" s="112"/>
-      <c r="O36" s="112"/>
-      <c r="P36" s="112"/>
-      <c r="Q36" s="112"/>
-      <c r="R36" s="112"/>
-      <c r="S36" s="112"/>
-      <c r="T36" s="113"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="116"/>
+      <c r="D36" s="117"/>
+      <c r="E36" s="118"/>
+      <c r="F36" s="118"/>
+      <c r="G36" s="118"/>
+      <c r="H36" s="118"/>
+      <c r="I36" s="118"/>
+      <c r="J36" s="118"/>
+      <c r="K36" s="118"/>
+      <c r="L36" s="102"/>
+      <c r="M36" s="102"/>
+      <c r="N36" s="102"/>
+      <c r="O36" s="102"/>
+      <c r="P36" s="102"/>
+      <c r="Q36" s="102"/>
+      <c r="R36" s="102"/>
+      <c r="S36" s="102"/>
+      <c r="T36" s="103"/>
     </row>
     <row r="37" spans="1:20" ht="93" customHeight="1" thickBot="1">
       <c r="A37" s="41">
         <v>26</v>
       </c>
-      <c r="B37" s="105"/>
-      <c r="C37" s="106"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="108"/>
-      <c r="F37" s="108"/>
-      <c r="G37" s="108"/>
-      <c r="H37" s="108"/>
-      <c r="I37" s="108"/>
-      <c r="J37" s="108"/>
-      <c r="K37" s="108"/>
-      <c r="L37" s="112"/>
-      <c r="M37" s="112"/>
-      <c r="N37" s="112"/>
-      <c r="O37" s="112"/>
-      <c r="P37" s="112"/>
-      <c r="Q37" s="112"/>
-      <c r="R37" s="112"/>
-      <c r="S37" s="112"/>
-      <c r="T37" s="113"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="116"/>
+      <c r="D37" s="117"/>
+      <c r="E37" s="118"/>
+      <c r="F37" s="118"/>
+      <c r="G37" s="118"/>
+      <c r="H37" s="118"/>
+      <c r="I37" s="118"/>
+      <c r="J37" s="118"/>
+      <c r="K37" s="118"/>
+      <c r="L37" s="102"/>
+      <c r="M37" s="102"/>
+      <c r="N37" s="102"/>
+      <c r="O37" s="102"/>
+      <c r="P37" s="102"/>
+      <c r="Q37" s="102"/>
+      <c r="R37" s="102"/>
+      <c r="S37" s="102"/>
+      <c r="T37" s="103"/>
     </row>
     <row r="38" spans="1:20" ht="113.1" customHeight="1" thickBot="1">
       <c r="A38" s="40">
         <v>27</v>
       </c>
-      <c r="B38" s="105"/>
-      <c r="C38" s="106"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="108"/>
-      <c r="F38" s="108"/>
-      <c r="G38" s="108"/>
-      <c r="H38" s="108"/>
-      <c r="I38" s="108"/>
-      <c r="J38" s="108"/>
-      <c r="K38" s="108"/>
-      <c r="L38" s="112"/>
-      <c r="M38" s="112"/>
-      <c r="N38" s="112"/>
-      <c r="O38" s="112"/>
-      <c r="P38" s="112"/>
-      <c r="Q38" s="112"/>
-      <c r="R38" s="112"/>
-      <c r="S38" s="112"/>
-      <c r="T38" s="113"/>
+      <c r="B38" s="115"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="117"/>
+      <c r="E38" s="118"/>
+      <c r="F38" s="118"/>
+      <c r="G38" s="118"/>
+      <c r="H38" s="118"/>
+      <c r="I38" s="118"/>
+      <c r="J38" s="118"/>
+      <c r="K38" s="118"/>
+      <c r="L38" s="102"/>
+      <c r="M38" s="102"/>
+      <c r="N38" s="102"/>
+      <c r="O38" s="102"/>
+      <c r="P38" s="102"/>
+      <c r="Q38" s="102"/>
+      <c r="R38" s="102"/>
+      <c r="S38" s="102"/>
+      <c r="T38" s="103"/>
     </row>
     <row r="39" spans="1:20" ht="27" customHeight="1" thickBot="1">
       <c r="A39" s="41">
         <v>28</v>
       </c>
-      <c r="B39" s="105"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="107"/>
-      <c r="E39" s="108"/>
-      <c r="F39" s="108"/>
-      <c r="G39" s="108"/>
-      <c r="H39" s="108"/>
-      <c r="I39" s="108"/>
-      <c r="J39" s="108"/>
-      <c r="K39" s="108"/>
-      <c r="L39" s="112"/>
-      <c r="M39" s="112"/>
-      <c r="N39" s="112"/>
-      <c r="O39" s="112"/>
-      <c r="P39" s="112"/>
-      <c r="Q39" s="112"/>
-      <c r="R39" s="112"/>
-      <c r="S39" s="112"/>
-      <c r="T39" s="113"/>
+      <c r="B39" s="115"/>
+      <c r="C39" s="116"/>
+      <c r="D39" s="117"/>
+      <c r="E39" s="118"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="118"/>
+      <c r="H39" s="118"/>
+      <c r="I39" s="118"/>
+      <c r="J39" s="118"/>
+      <c r="K39" s="118"/>
+      <c r="L39" s="102"/>
+      <c r="M39" s="102"/>
+      <c r="N39" s="102"/>
+      <c r="O39" s="102"/>
+      <c r="P39" s="102"/>
+      <c r="Q39" s="102"/>
+      <c r="R39" s="102"/>
+      <c r="S39" s="102"/>
+      <c r="T39" s="103"/>
     </row>
     <row r="40" spans="1:20" ht="56.45" customHeight="1" thickBot="1">
       <c r="A40" s="40">
         <v>29</v>
       </c>
-      <c r="B40" s="105"/>
-      <c r="C40" s="106"/>
-      <c r="D40" s="107"/>
-      <c r="E40" s="108"/>
-      <c r="F40" s="108"/>
-      <c r="G40" s="108"/>
-      <c r="H40" s="108"/>
-      <c r="I40" s="108"/>
-      <c r="J40" s="108"/>
-      <c r="K40" s="108"/>
-      <c r="L40" s="112"/>
-      <c r="M40" s="112"/>
-      <c r="N40" s="112"/>
-      <c r="O40" s="112"/>
-      <c r="P40" s="112"/>
-      <c r="Q40" s="112"/>
-      <c r="R40" s="112"/>
-      <c r="S40" s="112"/>
-      <c r="T40" s="113"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="116"/>
+      <c r="D40" s="117"/>
+      <c r="E40" s="118"/>
+      <c r="F40" s="118"/>
+      <c r="G40" s="118"/>
+      <c r="H40" s="118"/>
+      <c r="I40" s="118"/>
+      <c r="J40" s="118"/>
+      <c r="K40" s="118"/>
+      <c r="L40" s="102"/>
+      <c r="M40" s="102"/>
+      <c r="N40" s="102"/>
+      <c r="O40" s="102"/>
+      <c r="P40" s="102"/>
+      <c r="Q40" s="102"/>
+      <c r="R40" s="102"/>
+      <c r="S40" s="102"/>
+      <c r="T40" s="103"/>
     </row>
     <row r="41" spans="1:20" ht="71.099999999999994" customHeight="1" thickBot="1">
       <c r="A41" s="40">
         <v>30</v>
       </c>
-      <c r="B41" s="105"/>
-      <c r="C41" s="106"/>
-      <c r="D41" s="107"/>
-      <c r="E41" s="108"/>
-      <c r="F41" s="108"/>
-      <c r="G41" s="108"/>
-      <c r="H41" s="108"/>
-      <c r="I41" s="108"/>
-      <c r="J41" s="108"/>
-      <c r="K41" s="108"/>
-      <c r="L41" s="112"/>
-      <c r="M41" s="112"/>
-      <c r="N41" s="112"/>
-      <c r="O41" s="112"/>
-      <c r="P41" s="112"/>
-      <c r="Q41" s="112"/>
-      <c r="R41" s="112"/>
-      <c r="S41" s="112"/>
-      <c r="T41" s="113"/>
+      <c r="B41" s="115"/>
+      <c r="C41" s="116"/>
+      <c r="D41" s="117"/>
+      <c r="E41" s="118"/>
+      <c r="F41" s="118"/>
+      <c r="G41" s="118"/>
+      <c r="H41" s="118"/>
+      <c r="I41" s="118"/>
+      <c r="J41" s="118"/>
+      <c r="K41" s="118"/>
+      <c r="L41" s="102"/>
+      <c r="M41" s="102"/>
+      <c r="N41" s="102"/>
+      <c r="O41" s="102"/>
+      <c r="P41" s="102"/>
+      <c r="Q41" s="102"/>
+      <c r="R41" s="102"/>
+      <c r="S41" s="102"/>
+      <c r="T41" s="103"/>
     </row>
     <row r="42" spans="1:20" ht="270.60000000000002" customHeight="1" thickBot="1">
       <c r="A42" s="41">
         <v>31</v>
       </c>
-      <c r="B42" s="105"/>
-      <c r="C42" s="106"/>
-      <c r="D42" s="107"/>
-      <c r="E42" s="108"/>
-      <c r="F42" s="108"/>
-      <c r="G42" s="108"/>
-      <c r="H42" s="108"/>
-      <c r="I42" s="108"/>
-      <c r="J42" s="108"/>
-      <c r="K42" s="108"/>
-      <c r="L42" s="114"/>
-      <c r="M42" s="112"/>
-      <c r="N42" s="112"/>
-      <c r="O42" s="112"/>
-      <c r="P42" s="112"/>
-      <c r="Q42" s="112"/>
-      <c r="R42" s="112"/>
-      <c r="S42" s="112"/>
-      <c r="T42" s="113"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="116"/>
+      <c r="D42" s="117"/>
+      <c r="E42" s="118"/>
+      <c r="F42" s="118"/>
+      <c r="G42" s="118"/>
+      <c r="H42" s="118"/>
+      <c r="I42" s="118"/>
+      <c r="J42" s="118"/>
+      <c r="K42" s="118"/>
+      <c r="L42" s="166"/>
+      <c r="M42" s="102"/>
+      <c r="N42" s="102"/>
+      <c r="O42" s="102"/>
+      <c r="P42" s="102"/>
+      <c r="Q42" s="102"/>
+      <c r="R42" s="102"/>
+      <c r="S42" s="102"/>
+      <c r="T42" s="103"/>
     </row>
     <row r="43" spans="1:20" ht="167.1" customHeight="1" thickBot="1">
       <c r="A43" s="40">
         <v>32</v>
       </c>
-      <c r="B43" s="105"/>
-      <c r="C43" s="106"/>
-      <c r="D43" s="107"/>
-      <c r="E43" s="108"/>
-      <c r="F43" s="108"/>
-      <c r="G43" s="108"/>
-      <c r="H43" s="108"/>
-      <c r="I43" s="108"/>
-      <c r="J43" s="108"/>
-      <c r="K43" s="108"/>
-      <c r="L43" s="107"/>
-      <c r="M43" s="112"/>
-      <c r="N43" s="112"/>
-      <c r="O43" s="112"/>
-      <c r="P43" s="112"/>
-      <c r="Q43" s="112"/>
-      <c r="R43" s="112"/>
-      <c r="S43" s="112"/>
-      <c r="T43" s="113"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="116"/>
+      <c r="D43" s="117"/>
+      <c r="E43" s="118"/>
+      <c r="F43" s="118"/>
+      <c r="G43" s="118"/>
+      <c r="H43" s="118"/>
+      <c r="I43" s="118"/>
+      <c r="J43" s="118"/>
+      <c r="K43" s="118"/>
+      <c r="L43" s="117"/>
+      <c r="M43" s="102"/>
+      <c r="N43" s="102"/>
+      <c r="O43" s="102"/>
+      <c r="P43" s="102"/>
+      <c r="Q43" s="102"/>
+      <c r="R43" s="102"/>
+      <c r="S43" s="102"/>
+      <c r="T43" s="103"/>
     </row>
     <row r="44" spans="1:20" ht="86.1" customHeight="1" thickBot="1">
       <c r="A44" s="41">
         <v>33</v>
       </c>
-      <c r="B44" s="105"/>
-      <c r="C44" s="106"/>
-      <c r="D44" s="107"/>
-      <c r="E44" s="108"/>
-      <c r="F44" s="108"/>
-      <c r="G44" s="108"/>
-      <c r="H44" s="108"/>
-      <c r="I44" s="108"/>
-      <c r="J44" s="108"/>
-      <c r="K44" s="108"/>
-      <c r="L44" s="102"/>
-      <c r="M44" s="103"/>
-      <c r="N44" s="103"/>
-      <c r="O44" s="103"/>
-      <c r="P44" s="103"/>
-      <c r="Q44" s="103"/>
-      <c r="R44" s="103"/>
-      <c r="S44" s="103"/>
-      <c r="T44" s="104"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="116"/>
+      <c r="D44" s="117"/>
+      <c r="E44" s="118"/>
+      <c r="F44" s="118"/>
+      <c r="G44" s="118"/>
+      <c r="H44" s="118"/>
+      <c r="I44" s="118"/>
+      <c r="J44" s="118"/>
+      <c r="K44" s="118"/>
+      <c r="L44" s="163"/>
+      <c r="M44" s="164"/>
+      <c r="N44" s="164"/>
+      <c r="O44" s="164"/>
+      <c r="P44" s="164"/>
+      <c r="Q44" s="164"/>
+      <c r="R44" s="164"/>
+      <c r="S44" s="164"/>
+      <c r="T44" s="165"/>
     </row>
     <row r="45" spans="1:20" ht="44.45" customHeight="1" thickBot="1">
       <c r="A45" s="40">
         <v>34</v>
       </c>
-      <c r="B45" s="105"/>
-      <c r="C45" s="106"/>
-      <c r="D45" s="107"/>
-      <c r="E45" s="108"/>
-      <c r="F45" s="108"/>
-      <c r="G45" s="108"/>
-      <c r="H45" s="108"/>
-      <c r="I45" s="108"/>
-      <c r="J45" s="108"/>
-      <c r="K45" s="108"/>
-      <c r="L45" s="102"/>
-      <c r="M45" s="103"/>
-      <c r="N45" s="103"/>
-      <c r="O45" s="103"/>
-      <c r="P45" s="103"/>
-      <c r="Q45" s="103"/>
-      <c r="R45" s="103"/>
-      <c r="S45" s="103"/>
-      <c r="T45" s="104"/>
+      <c r="B45" s="115"/>
+      <c r="C45" s="116"/>
+      <c r="D45" s="117"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="118"/>
+      <c r="I45" s="118"/>
+      <c r="J45" s="118"/>
+      <c r="K45" s="118"/>
+      <c r="L45" s="163"/>
+      <c r="M45" s="164"/>
+      <c r="N45" s="164"/>
+      <c r="O45" s="164"/>
+      <c r="P45" s="164"/>
+      <c r="Q45" s="164"/>
+      <c r="R45" s="164"/>
+      <c r="S45" s="164"/>
+      <c r="T45" s="165"/>
     </row>
     <row r="46" spans="1:20" ht="67.349999999999994" customHeight="1" thickBot="1">
       <c r="A46" s="40">
         <v>35</v>
       </c>
-      <c r="B46" s="105"/>
-      <c r="C46" s="106"/>
-      <c r="D46" s="107"/>
-      <c r="E46" s="108"/>
-      <c r="F46" s="108"/>
-      <c r="G46" s="108"/>
-      <c r="H46" s="108"/>
-      <c r="I46" s="108"/>
-      <c r="J46" s="108"/>
-      <c r="K46" s="108"/>
-      <c r="L46" s="103"/>
-      <c r="M46" s="103"/>
-      <c r="N46" s="103"/>
-      <c r="O46" s="103"/>
-      <c r="P46" s="103"/>
-      <c r="Q46" s="103"/>
-      <c r="R46" s="103"/>
-      <c r="S46" s="103"/>
-      <c r="T46" s="104"/>
+      <c r="B46" s="115"/>
+      <c r="C46" s="116"/>
+      <c r="D46" s="117"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="118"/>
+      <c r="G46" s="118"/>
+      <c r="H46" s="118"/>
+      <c r="I46" s="118"/>
+      <c r="J46" s="118"/>
+      <c r="K46" s="118"/>
+      <c r="L46" s="164"/>
+      <c r="M46" s="164"/>
+      <c r="N46" s="164"/>
+      <c r="O46" s="164"/>
+      <c r="P46" s="164"/>
+      <c r="Q46" s="164"/>
+      <c r="R46" s="164"/>
+      <c r="S46" s="164"/>
+      <c r="T46" s="165"/>
     </row>
     <row r="47" spans="1:20" ht="60" customHeight="1" thickBot="1">
       <c r="A47" s="41">
         <v>36</v>
       </c>
-      <c r="B47" s="105"/>
-      <c r="C47" s="106"/>
-      <c r="D47" s="107"/>
-      <c r="E47" s="108"/>
-      <c r="F47" s="108"/>
-      <c r="G47" s="108"/>
-      <c r="H47" s="108"/>
-      <c r="I47" s="108"/>
-      <c r="J47" s="108"/>
-      <c r="K47" s="108"/>
-      <c r="L47" s="103"/>
-      <c r="M47" s="103"/>
-      <c r="N47" s="103"/>
-      <c r="O47" s="103"/>
-      <c r="P47" s="103"/>
-      <c r="Q47" s="103"/>
-      <c r="R47" s="103"/>
-      <c r="S47" s="103"/>
-      <c r="T47" s="104"/>
+      <c r="B47" s="115"/>
+      <c r="C47" s="116"/>
+      <c r="D47" s="117"/>
+      <c r="E47" s="118"/>
+      <c r="F47" s="118"/>
+      <c r="G47" s="118"/>
+      <c r="H47" s="118"/>
+      <c r="I47" s="118"/>
+      <c r="J47" s="118"/>
+      <c r="K47" s="118"/>
+      <c r="L47" s="164"/>
+      <c r="M47" s="164"/>
+      <c r="N47" s="164"/>
+      <c r="O47" s="164"/>
+      <c r="P47" s="164"/>
+      <c r="Q47" s="164"/>
+      <c r="R47" s="164"/>
+      <c r="S47" s="164"/>
+      <c r="T47" s="165"/>
     </row>
     <row r="48" spans="1:20" ht="66" customHeight="1" thickBot="1">
       <c r="A48" s="40">
         <v>37</v>
       </c>
-      <c r="B48" s="105"/>
-      <c r="C48" s="106"/>
-      <c r="D48" s="107"/>
-      <c r="E48" s="108"/>
-      <c r="F48" s="108"/>
-      <c r="G48" s="108"/>
-      <c r="H48" s="108"/>
-      <c r="I48" s="108"/>
-      <c r="J48" s="108"/>
-      <c r="K48" s="108"/>
-      <c r="L48" s="106"/>
-      <c r="M48" s="106"/>
-      <c r="N48" s="106"/>
-      <c r="O48" s="106"/>
-      <c r="P48" s="106"/>
-      <c r="Q48" s="106"/>
-      <c r="R48" s="106"/>
-      <c r="S48" s="106"/>
-      <c r="T48" s="109"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="116"/>
+      <c r="D48" s="117"/>
+      <c r="E48" s="118"/>
+      <c r="F48" s="118"/>
+      <c r="G48" s="118"/>
+      <c r="H48" s="118"/>
+      <c r="I48" s="118"/>
+      <c r="J48" s="118"/>
+      <c r="K48" s="118"/>
+      <c r="L48" s="116"/>
+      <c r="M48" s="116"/>
+      <c r="N48" s="116"/>
+      <c r="O48" s="116"/>
+      <c r="P48" s="116"/>
+      <c r="Q48" s="116"/>
+      <c r="R48" s="116"/>
+      <c r="S48" s="116"/>
+      <c r="T48" s="167"/>
     </row>
     <row r="49" spans="1:20" ht="80.45" customHeight="1" thickBot="1">
       <c r="A49" s="41">
         <v>38</v>
       </c>
-      <c r="B49" s="105"/>
-      <c r="C49" s="106"/>
-      <c r="D49" s="107"/>
-      <c r="E49" s="108"/>
-      <c r="F49" s="108"/>
-      <c r="G49" s="108"/>
-      <c r="H49" s="108"/>
-      <c r="I49" s="108"/>
-      <c r="J49" s="108"/>
-      <c r="K49" s="108"/>
-      <c r="L49" s="106"/>
-      <c r="M49" s="106"/>
-      <c r="N49" s="106"/>
-      <c r="O49" s="106"/>
-      <c r="P49" s="106"/>
-      <c r="Q49" s="106"/>
-      <c r="R49" s="106"/>
-      <c r="S49" s="106"/>
-      <c r="T49" s="109"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="116"/>
+      <c r="D49" s="117"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="118"/>
+      <c r="L49" s="116"/>
+      <c r="M49" s="116"/>
+      <c r="N49" s="116"/>
+      <c r="O49" s="116"/>
+      <c r="P49" s="116"/>
+      <c r="Q49" s="116"/>
+      <c r="R49" s="116"/>
+      <c r="S49" s="116"/>
+      <c r="T49" s="167"/>
     </row>
     <row r="50" spans="1:20" ht="29.1" customHeight="1" thickBot="1">
       <c r="A50" s="40">
         <v>39</v>
       </c>
-      <c r="B50" s="105"/>
-      <c r="C50" s="106"/>
-      <c r="D50" s="108"/>
-      <c r="E50" s="108"/>
-      <c r="F50" s="108"/>
-      <c r="G50" s="108"/>
-      <c r="H50" s="108"/>
-      <c r="I50" s="108"/>
-      <c r="J50" s="108"/>
-      <c r="K50" s="108"/>
-      <c r="L50" s="106"/>
-      <c r="M50" s="106"/>
-      <c r="N50" s="106"/>
-      <c r="O50" s="106"/>
-      <c r="P50" s="106"/>
-      <c r="Q50" s="106"/>
-      <c r="R50" s="106"/>
-      <c r="S50" s="106"/>
-      <c r="T50" s="109"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="116"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="118"/>
+      <c r="F50" s="118"/>
+      <c r="G50" s="118"/>
+      <c r="H50" s="118"/>
+      <c r="I50" s="118"/>
+      <c r="J50" s="118"/>
+      <c r="K50" s="118"/>
+      <c r="L50" s="116"/>
+      <c r="M50" s="116"/>
+      <c r="N50" s="116"/>
+      <c r="O50" s="116"/>
+      <c r="P50" s="116"/>
+      <c r="Q50" s="116"/>
+      <c r="R50" s="116"/>
+      <c r="S50" s="116"/>
+      <c r="T50" s="167"/>
     </row>
     <row r="51" spans="1:20" ht="13.5" thickBot="1">
       <c r="A51" s="40">
         <v>40</v>
       </c>
-      <c r="B51" s="105"/>
-      <c r="C51" s="106"/>
-      <c r="D51" s="107"/>
-      <c r="E51" s="108"/>
-      <c r="F51" s="108"/>
-      <c r="G51" s="108"/>
-      <c r="H51" s="108"/>
-      <c r="I51" s="108"/>
-      <c r="J51" s="108"/>
-      <c r="K51" s="108"/>
-      <c r="L51" s="106"/>
-      <c r="M51" s="106"/>
-      <c r="N51" s="106"/>
-      <c r="O51" s="106"/>
-      <c r="P51" s="106"/>
-      <c r="Q51" s="106"/>
-      <c r="R51" s="106"/>
-      <c r="S51" s="106"/>
-      <c r="T51" s="109"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="116"/>
+      <c r="D51" s="117"/>
+      <c r="E51" s="118"/>
+      <c r="F51" s="118"/>
+      <c r="G51" s="118"/>
+      <c r="H51" s="118"/>
+      <c r="I51" s="118"/>
+      <c r="J51" s="118"/>
+      <c r="K51" s="118"/>
+      <c r="L51" s="116"/>
+      <c r="M51" s="116"/>
+      <c r="N51" s="116"/>
+      <c r="O51" s="116"/>
+      <c r="P51" s="116"/>
+      <c r="Q51" s="116"/>
+      <c r="R51" s="116"/>
+      <c r="S51" s="116"/>
+      <c r="T51" s="167"/>
     </row>
     <row r="52" spans="1:20" ht="49.35" customHeight="1" thickBot="1">
       <c r="A52" s="41">
         <v>41</v>
       </c>
-      <c r="B52" s="105"/>
-      <c r="C52" s="106"/>
-      <c r="D52" s="108"/>
-      <c r="E52" s="108"/>
-      <c r="F52" s="108"/>
-      <c r="G52" s="108"/>
-      <c r="H52" s="108"/>
-      <c r="I52" s="108"/>
-      <c r="J52" s="108"/>
-      <c r="K52" s="108"/>
-      <c r="L52" s="103"/>
-      <c r="M52" s="103"/>
-      <c r="N52" s="103"/>
-      <c r="O52" s="103"/>
-      <c r="P52" s="103"/>
-      <c r="Q52" s="103"/>
-      <c r="R52" s="103"/>
-      <c r="S52" s="103"/>
-      <c r="T52" s="104"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="116"/>
+      <c r="D52" s="118"/>
+      <c r="E52" s="118"/>
+      <c r="F52" s="118"/>
+      <c r="G52" s="118"/>
+      <c r="H52" s="118"/>
+      <c r="I52" s="118"/>
+      <c r="J52" s="118"/>
+      <c r="K52" s="118"/>
+      <c r="L52" s="164"/>
+      <c r="M52" s="164"/>
+      <c r="N52" s="164"/>
+      <c r="O52" s="164"/>
+      <c r="P52" s="164"/>
+      <c r="Q52" s="164"/>
+      <c r="R52" s="164"/>
+      <c r="S52" s="164"/>
+      <c r="T52" s="165"/>
     </row>
     <row r="53" spans="1:20" ht="48" customHeight="1" thickBot="1">
       <c r="A53" s="40">
         <v>42</v>
       </c>
-      <c r="B53" s="105"/>
-      <c r="C53" s="106"/>
-      <c r="D53" s="107"/>
-      <c r="E53" s="108"/>
-      <c r="F53" s="108"/>
-      <c r="G53" s="108"/>
-      <c r="H53" s="108"/>
-      <c r="I53" s="108"/>
-      <c r="J53" s="108"/>
-      <c r="K53" s="108"/>
-      <c r="L53" s="103"/>
-      <c r="M53" s="103"/>
-      <c r="N53" s="103"/>
-      <c r="O53" s="103"/>
-      <c r="P53" s="103"/>
-      <c r="Q53" s="103"/>
-      <c r="R53" s="103"/>
-      <c r="S53" s="103"/>
-      <c r="T53" s="104"/>
+      <c r="B53" s="115"/>
+      <c r="C53" s="116"/>
+      <c r="D53" s="117"/>
+      <c r="E53" s="118"/>
+      <c r="F53" s="118"/>
+      <c r="G53" s="118"/>
+      <c r="H53" s="118"/>
+      <c r="I53" s="118"/>
+      <c r="J53" s="118"/>
+      <c r="K53" s="118"/>
+      <c r="L53" s="164"/>
+      <c r="M53" s="164"/>
+      <c r="N53" s="164"/>
+      <c r="O53" s="164"/>
+      <c r="P53" s="164"/>
+      <c r="Q53" s="164"/>
+      <c r="R53" s="164"/>
+      <c r="S53" s="164"/>
+      <c r="T53" s="165"/>
     </row>
     <row r="54" spans="1:20" ht="105" customHeight="1" thickBot="1">
       <c r="A54" s="41">
         <v>43</v>
       </c>
-      <c r="B54" s="105"/>
-      <c r="C54" s="106"/>
-      <c r="D54" s="107"/>
-      <c r="E54" s="108"/>
-      <c r="F54" s="108"/>
-      <c r="G54" s="108"/>
-      <c r="H54" s="108"/>
-      <c r="I54" s="108"/>
-      <c r="J54" s="108"/>
-      <c r="K54" s="108"/>
-      <c r="L54" s="106"/>
-      <c r="M54" s="106"/>
-      <c r="N54" s="106"/>
-      <c r="O54" s="106"/>
-      <c r="P54" s="106"/>
-      <c r="Q54" s="106"/>
-      <c r="R54" s="106"/>
-      <c r="S54" s="106"/>
-      <c r="T54" s="109"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="116"/>
+      <c r="D54" s="117"/>
+      <c r="E54" s="118"/>
+      <c r="F54" s="118"/>
+      <c r="G54" s="118"/>
+      <c r="H54" s="118"/>
+      <c r="I54" s="118"/>
+      <c r="J54" s="118"/>
+      <c r="K54" s="118"/>
+      <c r="L54" s="116"/>
+      <c r="M54" s="116"/>
+      <c r="N54" s="116"/>
+      <c r="O54" s="116"/>
+      <c r="P54" s="116"/>
+      <c r="Q54" s="116"/>
+      <c r="R54" s="116"/>
+      <c r="S54" s="116"/>
+      <c r="T54" s="167"/>
     </row>
     <row r="55" spans="1:20" ht="39" customHeight="1" thickBot="1">
       <c r="A55" s="40">
         <v>44</v>
       </c>
-      <c r="B55" s="105"/>
-      <c r="C55" s="106"/>
-      <c r="D55" s="108"/>
-      <c r="E55" s="108"/>
-      <c r="F55" s="108"/>
-      <c r="G55" s="108"/>
-      <c r="H55" s="108"/>
-      <c r="I55" s="108"/>
-      <c r="J55" s="108"/>
-      <c r="K55" s="108"/>
-      <c r="L55" s="106"/>
-      <c r="M55" s="106"/>
-      <c r="N55" s="106"/>
-      <c r="O55" s="106"/>
-      <c r="P55" s="106"/>
-      <c r="Q55" s="106"/>
-      <c r="R55" s="106"/>
-      <c r="S55" s="106"/>
-      <c r="T55" s="109"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="116"/>
+      <c r="D55" s="118"/>
+      <c r="E55" s="118"/>
+      <c r="F55" s="118"/>
+      <c r="G55" s="118"/>
+      <c r="H55" s="118"/>
+      <c r="I55" s="118"/>
+      <c r="J55" s="118"/>
+      <c r="K55" s="118"/>
+      <c r="L55" s="116"/>
+      <c r="M55" s="116"/>
+      <c r="N55" s="116"/>
+      <c r="O55" s="116"/>
+      <c r="P55" s="116"/>
+      <c r="Q55" s="116"/>
+      <c r="R55" s="116"/>
+      <c r="S55" s="116"/>
+      <c r="T55" s="167"/>
     </row>
     <row r="56" spans="1:20" ht="44.1" customHeight="1" thickBot="1">
       <c r="A56" s="40">
         <v>45</v>
       </c>
-      <c r="B56" s="105"/>
-      <c r="C56" s="106"/>
-      <c r="D56" s="107"/>
-      <c r="E56" s="108"/>
-      <c r="F56" s="108"/>
-      <c r="G56" s="108"/>
-      <c r="H56" s="108"/>
-      <c r="I56" s="108"/>
-      <c r="J56" s="108"/>
-      <c r="K56" s="108"/>
-      <c r="L56" s="103"/>
-      <c r="M56" s="103"/>
-      <c r="N56" s="103"/>
-      <c r="O56" s="103"/>
-      <c r="P56" s="103"/>
-      <c r="Q56" s="103"/>
-      <c r="R56" s="103"/>
-      <c r="S56" s="103"/>
-      <c r="T56" s="104"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="116"/>
+      <c r="D56" s="117"/>
+      <c r="E56" s="118"/>
+      <c r="F56" s="118"/>
+      <c r="G56" s="118"/>
+      <c r="H56" s="118"/>
+      <c r="I56" s="118"/>
+      <c r="J56" s="118"/>
+      <c r="K56" s="118"/>
+      <c r="L56" s="164"/>
+      <c r="M56" s="164"/>
+      <c r="N56" s="164"/>
+      <c r="O56" s="164"/>
+      <c r="P56" s="164"/>
+      <c r="Q56" s="164"/>
+      <c r="R56" s="164"/>
+      <c r="S56" s="164"/>
+      <c r="T56" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="155">
+    <mergeCell ref="L44:T44"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:K53"/>
+    <mergeCell ref="L53:T53"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:K46"/>
+    <mergeCell ref="L46:T46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:K47"/>
+    <mergeCell ref="L47:T47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:K48"/>
+    <mergeCell ref="L48:T48"/>
+    <mergeCell ref="L52:T52"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:K49"/>
+    <mergeCell ref="L49:T49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:K50"/>
+    <mergeCell ref="L50:T50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:K51"/>
+    <mergeCell ref="L51:T51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="D56:K56"/>
+    <mergeCell ref="L56:T56"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:K54"/>
+    <mergeCell ref="L54:T54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:K55"/>
+    <mergeCell ref="L55:T55"/>
+    <mergeCell ref="D52:K52"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:K45"/>
+    <mergeCell ref="L45:T45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="L38:T38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="L39:T39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:K40"/>
+    <mergeCell ref="L40:T40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="L41:T41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:K42"/>
+    <mergeCell ref="L42:T42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:K43"/>
+    <mergeCell ref="L43:T43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:K44"/>
+    <mergeCell ref="D35:K35"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:K11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:K36"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D24:K24"/>
+    <mergeCell ref="D25:K25"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:O1"/>
+    <mergeCell ref="C2:O2"/>
+    <mergeCell ref="C3:O3"/>
+    <mergeCell ref="C7:L7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="L12:T12"/>
+    <mergeCell ref="L13:T13"/>
+    <mergeCell ref="L15:T15"/>
+    <mergeCell ref="C9:L9"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="D12:K12"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="L11:T11"/>
+    <mergeCell ref="D14:K14"/>
+    <mergeCell ref="L36:T36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="L37:T37"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="L16:T16"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="L33:T33"/>
+    <mergeCell ref="D28:K28"/>
+    <mergeCell ref="L28:T28"/>
+    <mergeCell ref="D29:K29"/>
+    <mergeCell ref="L29:T29"/>
+    <mergeCell ref="D30:K30"/>
+    <mergeCell ref="L27:T27"/>
+    <mergeCell ref="L34:T34"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="L25:T25"/>
+    <mergeCell ref="D26:K26"/>
+    <mergeCell ref="D22:K22"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D34:K34"/>
+    <mergeCell ref="D27:K27"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="L35:T35"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D15:K15"/>
@@ -4351,137 +4478,6 @@
     <mergeCell ref="L30:T30"/>
     <mergeCell ref="L26:T26"/>
     <mergeCell ref="L24:T24"/>
-    <mergeCell ref="L25:T25"/>
-    <mergeCell ref="D26:K26"/>
-    <mergeCell ref="D22:K22"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D34:K34"/>
-    <mergeCell ref="D27:K27"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="L36:T36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="L37:T37"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="D18:K18"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="L16:T16"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="L33:T33"/>
-    <mergeCell ref="D28:K28"/>
-    <mergeCell ref="L28:T28"/>
-    <mergeCell ref="D29:K29"/>
-    <mergeCell ref="L29:T29"/>
-    <mergeCell ref="D30:K30"/>
-    <mergeCell ref="L27:T27"/>
-    <mergeCell ref="L34:T34"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="L12:T12"/>
-    <mergeCell ref="L13:T13"/>
-    <mergeCell ref="L15:T15"/>
-    <mergeCell ref="C9:L9"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="D12:K12"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="L11:T11"/>
-    <mergeCell ref="D14:K14"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:O1"/>
-    <mergeCell ref="C2:O2"/>
-    <mergeCell ref="C3:O3"/>
-    <mergeCell ref="C7:L7"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D44:K44"/>
-    <mergeCell ref="D35:K35"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:K11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D19:K19"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:K36"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D24:K24"/>
-    <mergeCell ref="D25:K25"/>
-    <mergeCell ref="D52:K52"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:K45"/>
-    <mergeCell ref="L45:T45"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:K38"/>
-    <mergeCell ref="L38:T38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:K39"/>
-    <mergeCell ref="L39:T39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:K40"/>
-    <mergeCell ref="L40:T40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="L41:T41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:K42"/>
-    <mergeCell ref="L42:T42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:K43"/>
-    <mergeCell ref="L43:T43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="D56:K56"/>
-    <mergeCell ref="L56:T56"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:K54"/>
-    <mergeCell ref="L54:T54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:K55"/>
-    <mergeCell ref="L55:T55"/>
-    <mergeCell ref="L44:T44"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:K53"/>
-    <mergeCell ref="L53:T53"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:K46"/>
-    <mergeCell ref="L46:T46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:K47"/>
-    <mergeCell ref="L47:T47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:K48"/>
-    <mergeCell ref="L48:T48"/>
-    <mergeCell ref="L52:T52"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:K49"/>
-    <mergeCell ref="L49:T49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:K50"/>
-    <mergeCell ref="L50:T50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:K51"/>
-    <mergeCell ref="L51:T51"/>
-    <mergeCell ref="B52:C52"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.66" right="0.68" top="0.42" bottom="0.17" header="0" footer="0"/>

</xml_diff>